<commit_message>
Working copy with excel and navigation changes
</commit_message>
<xml_diff>
--- a/ConfigFile/TestDataFile.xlsx
+++ b/ConfigFile/TestDataFile.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\AllSelCSharpProjects\POC\DemoProject\DemoProject\TestData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\AllSelCSharpProjects\POM_Proj\ProjectPOC\ConfigFile\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="18">
   <si>
     <t>FirstName</t>
   </si>
@@ -59,9 +59,6 @@
     <t>Sharma</t>
   </si>
   <si>
-    <t>ankita.sharma@gmail.com</t>
-  </si>
-  <si>
     <t>System@123</t>
   </si>
   <si>
@@ -75,6 +72,12 @@
   </si>
   <si>
     <t>Speciality</t>
+  </si>
+  <si>
+    <t>ankita.singh@gmail.com</t>
+  </si>
+  <si>
+    <t>Agasthya@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -406,7 +409,7 @@
   <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="J1" sqref="J1"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -452,7 +455,7 @@
         <v>8</v>
       </c>
       <c r="J1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.35">
@@ -463,34 +466,35 @@
         <v>10</v>
       </c>
       <c r="C2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D2" t="s">
+      <c r="F2" t="s">
         <v>11</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="G2" t="s">
         <v>12</v>
-      </c>
-      <c r="F2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G2" t="s">
-        <v>13</v>
       </c>
       <c r="H2">
         <v>201306</v>
       </c>
       <c r="I2" t="s">
+        <v>13</v>
+      </c>
+      <c r="J2" t="s">
         <v>14</v>
-      </c>
-      <c r="J2" t="s">
-        <v>15</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1"/>
-    <hyperlink ref="E2" r:id="rId2"/>
+    <hyperlink ref="E2" r:id="rId1"/>
+    <hyperlink ref="D2" r:id="rId2"/>
+    <hyperlink ref="C2" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Running code - but reading data from RegisterUser
</commit_message>
<xml_diff>
--- a/ConfigFile/TestDataFile.xlsx
+++ b/ConfigFile/TestDataFile.xlsx
@@ -72,13 +72,13 @@
     <t>Agasthya@gmail.com</t>
   </si>
   <si>
-    <t>Anju</t>
-  </si>
-  <si>
-    <t>Singh</t>
-  </si>
-  <si>
-    <t>Anjusingh@gmail.com</t>
+    <t>Shruti</t>
+  </si>
+  <si>
+    <t>Malhotra</t>
+  </si>
+  <si>
+    <t>shruti.malhotra@gmail.com</t>
   </si>
 </sst>
 </file>

</xml_diff>